<commit_message>
Adding esp32 and other stuff
</commit_message>
<xml_diff>
--- a/RGBEMP ARK Control Board/ARK BOM.xlsx
+++ b/RGBEMP ARK Control Board/ARK BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monke\Documents\GitHub\PCB-File-System\RGBEMP ARK Control Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506E01C1-87BE-43E6-8E2C-FA4F5A33BB1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{233C1447-89F6-4AF8-9FE1-90F51D5D0A53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="24516" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
   <si>
     <t>Type</t>
   </si>
@@ -66,18 +66,9 @@
     <t>Digi-Key per Board</t>
   </si>
   <si>
-    <t xml:space="preserve">ESP-WROOM-02 (4MB) </t>
-  </si>
-  <si>
     <t>uController</t>
   </si>
   <si>
-    <t>https://www.mouser.com/datasheet/2/891/0c-esp-wroom-02_datasheet_en-1365805.pdf</t>
-  </si>
-  <si>
-    <t>1904-1018-1-ND</t>
-  </si>
-  <si>
     <t>12k Ohm</t>
   </si>
   <si>
@@ -105,9 +96,6 @@
     <t>0.300/0.11720/0.04906</t>
   </si>
   <si>
-    <t xml:space="preserve">356-ESPWROOM-024MB </t>
-  </si>
-  <si>
     <t>330 Ohm</t>
   </si>
   <si>
@@ -178,16 +166,70 @@
   </si>
   <si>
     <t>0.346/0.1960/0.09950</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schottcky </t>
+  </si>
+  <si>
+    <t>NPN Trans</t>
+  </si>
+  <si>
+    <t>our cost</t>
+  </si>
+  <si>
+    <t>pcbway cost</t>
+  </si>
+  <si>
+    <t>UART Bridge</t>
+  </si>
+  <si>
+    <t>3x 12k R</t>
+  </si>
+  <si>
+    <t>1x 330 R</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>1x 0.1uF C</t>
+  </si>
+  <si>
+    <t>1x 1uF EC</t>
+  </si>
+  <si>
+    <t>ESP32-WROVER-IB</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/datasheet/2/891/esp32-wrover-b_datasheet_en-1384674.pdf</t>
+  </si>
+  <si>
+    <t>356-ESP32-WROVER-IB</t>
+  </si>
+  <si>
+    <t>4.5(1)</t>
+  </si>
+  <si>
+    <t>4.8/(1)</t>
+  </si>
+  <si>
+    <t>1904-1035-1-ND</t>
+  </si>
+  <si>
+    <t>90 Degree Neopixel</t>
+  </si>
+  <si>
+    <t>IC</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/32890356895.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -223,18 +265,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -346,11 +376,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -370,7 +399,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -382,20 +410,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="8" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -416,7 +430,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -430,7 +444,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -457,7 +471,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -482,7 +496,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -498,9 +512,39 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
@@ -775,7 +819,7 @@
   </sheetPr>
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -799,7 +843,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="13.2">
-      <c r="A1" s="16"/>
+      <c r="A1" s="15"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,197 +883,199 @@
       </c>
     </row>
     <row r="2" spans="1:15" ht="13.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="72">
+        <v>1</v>
+      </c>
+      <c r="D2" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="73"/>
+      <c r="F2" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="76" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="77" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="74"/>
+      <c r="K2" s="79" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="80"/>
+      <c r="M2" s="78" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="82"/>
+    </row>
+    <row r="3" spans="1:15" ht="13.2">
+      <c r="A3" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="4">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="18" t="s">
+      <c r="B3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="9" t="s">
+      <c r="C3" s="19"/>
+      <c r="D3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="17"/>
+      <c r="F3" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="25"/>
+      <c r="M3" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="28"/>
+    </row>
+    <row r="4" spans="1:15" ht="13.2">
+      <c r="A4" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="30"/>
+      <c r="F4" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="19">
-        <v>3</v>
-      </c>
-      <c r="L2" s="20">
-        <v>3</v>
-      </c>
-      <c r="M2" s="21">
-        <v>3</v>
-      </c>
-      <c r="N2" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="13.2">
-      <c r="A3" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="24"/>
-      <c r="F3" s="33" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="27"/>
-      <c r="K3" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="32"/>
-      <c r="M3" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="35"/>
-    </row>
-    <row r="4" spans="1:15" ht="13.2">
-      <c r="A4" s="36" t="s">
+      <c r="I4" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="37"/>
-      <c r="F4" s="41" t="s">
+      <c r="J4" s="33"/>
+      <c r="K4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="47" t="s">
+      <c r="L4" s="39"/>
+      <c r="M4" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="42" t="s">
+      <c r="N4" s="41"/>
+    </row>
+    <row r="5" spans="1:15" ht="13.2">
+      <c r="A5" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I4" s="43" t="s">
+      <c r="B5" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="J4" s="40"/>
-      <c r="K4" s="45" t="s">
+      <c r="C5" s="45"/>
+      <c r="D5" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="46"/>
-      <c r="M4" s="44" t="s">
+      <c r="E5" s="43"/>
+      <c r="F5" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="48"/>
-    </row>
-    <row r="5" spans="1:15" ht="13.2">
-      <c r="A5" s="49" t="s">
+      <c r="G5" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="I5" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="52"/>
-      <c r="D5" s="51" t="s">
+      <c r="J5" s="46"/>
+      <c r="K5" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="50"/>
-      <c r="F5" s="54" t="s">
+      <c r="L5" s="53"/>
+      <c r="M5" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="56" t="s">
+      <c r="N5" s="54"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" spans="1:15" ht="13.2">
+      <c r="A6" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="B6" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="53"/>
-      <c r="K5" s="59" t="s">
+      <c r="C6" s="58"/>
+      <c r="D6" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="60"/>
-      <c r="M5" s="58" t="s">
+      <c r="E6" s="56"/>
+      <c r="F6" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="61"/>
-      <c r="O5" s="5"/>
-    </row>
-    <row r="6" spans="1:15" ht="13.2">
-      <c r="A6" s="62" t="s">
+      <c r="G6" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="H6" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="65" t="s">
+      <c r="I6" s="63" t="s">
         <v>43</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="67" t="s">
+      <c r="J6" s="59"/>
+      <c r="K6" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="68" t="s">
+      <c r="L6" s="66"/>
+      <c r="M6" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" s="66"/>
-      <c r="K6" s="72" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="73"/>
-      <c r="M6" s="71" t="s">
-        <v>49</v>
-      </c>
-      <c r="N6" s="74"/>
+      <c r="N6" s="67"/>
       <c r="O6" s="5"/>
     </row>
     <row r="7" spans="1:15" ht="13.2">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3"/>
+      <c r="A7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="7"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="7" t="s">
+        <v>64</v>
+      </c>
       <c r="G7" s="8"/>
       <c r="H7" s="9"/>
       <c r="I7" s="10"/>
       <c r="J7" s="6"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
       <c r="N7" s="10"/>
       <c r="O7" s="5"/>
     </row>
@@ -1038,15 +1084,15 @@
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="3"/>
-      <c r="E8" s="15"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
       <c r="H8" s="9"/>
       <c r="I8" s="10"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="13"/>
-      <c r="M8" s="14"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="13"/>
       <c r="N8" s="10"/>
       <c r="O8" s="5"/>
     </row>
@@ -1055,15 +1101,15 @@
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="15"/>
+      <c r="E9" s="14"/>
       <c r="F9" s="7"/>
       <c r="G9" s="8"/>
       <c r="H9" s="9"/>
       <c r="I9" s="10"/>
       <c r="J9" s="6"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="13"/>
       <c r="N9" s="10"/>
       <c r="O9" s="5"/>
     </row>
@@ -1072,15 +1118,15 @@
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="15"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="9"/>
       <c r="I10" s="10"/>
       <c r="J10" s="6"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="13"/>
-      <c r="M10" s="14"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13"/>
       <c r="N10" s="10"/>
       <c r="O10" s="5"/>
     </row>
@@ -1089,15 +1135,15 @@
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="15"/>
+      <c r="E11" s="14"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="9"/>
       <c r="I11" s="10"/>
       <c r="J11" s="6"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="13"/>
       <c r="N11" s="10"/>
       <c r="O11" s="5"/>
     </row>
@@ -1106,15 +1152,15 @@
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="15"/>
+      <c r="E12" s="14"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8"/>
       <c r="H12" s="9"/>
       <c r="I12" s="10"/>
       <c r="J12" s="6"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
-      <c r="M12" s="14"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="13"/>
       <c r="N12" s="10"/>
       <c r="O12" s="5"/>
     </row>
@@ -1123,15 +1169,15 @@
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="15"/>
+      <c r="E13" s="14"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="H13" s="9"/>
       <c r="I13" s="10"/>
       <c r="J13" s="6"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="13"/>
       <c r="N13" s="10"/>
       <c r="O13" s="5"/>
     </row>
@@ -1140,32 +1186,34 @@
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="15"/>
+      <c r="E14" s="14"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="9"/>
       <c r="I14" s="10"/>
       <c r="J14" s="6"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="13"/>
-      <c r="M14" s="14"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="10"/>
       <c r="O14" s="5"/>
     </row>
     <row r="15" spans="1:15" ht="13.2">
-      <c r="A15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>53</v>
+      </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="15"/>
+      <c r="E15" s="14"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="H15" s="9"/>
       <c r="I15" s="10"/>
       <c r="J15" s="6"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="13"/>
-      <c r="M15" s="14"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="13"/>
       <c r="N15" s="10"/>
       <c r="O15" s="5"/>
     </row>
@@ -1174,15 +1222,15 @@
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="15"/>
+      <c r="E16" s="14"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8"/>
       <c r="H16" s="9"/>
       <c r="I16" s="10"/>
       <c r="J16" s="6"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="14"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
       <c r="N16" s="10"/>
       <c r="O16" s="5"/>
     </row>
@@ -1191,15 +1239,15 @@
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="3"/>
-      <c r="E17" s="15"/>
+      <c r="E17" s="14"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="9"/>
       <c r="I17" s="10"/>
       <c r="J17" s="6"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="14"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="13"/>
       <c r="N17" s="10"/>
       <c r="O17" s="5"/>
     </row>
@@ -1208,15 +1256,15 @@
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="15"/>
+      <c r="E18" s="14"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="H18" s="9"/>
       <c r="I18" s="10"/>
       <c r="J18" s="6"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="14"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
       <c r="N18" s="10"/>
       <c r="O18" s="5"/>
     </row>
@@ -1225,15 +1273,15 @@
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="15"/>
+      <c r="E19" s="14"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="9"/>
       <c r="I19" s="10"/>
       <c r="J19" s="6"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="14"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="13"/>
       <c r="N19" s="10"/>
       <c r="O19" s="5"/>
     </row>
@@ -1242,15 +1290,15 @@
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="15"/>
+      <c r="E20" s="14"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8"/>
       <c r="H20" s="9"/>
       <c r="I20" s="10"/>
       <c r="J20" s="6"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="14"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="13"/>
       <c r="N20" s="10"/>
       <c r="O20" s="5"/>
     </row>
@@ -1259,23 +1307,27 @@
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="15"/>
+      <c r="E21" s="14"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
       <c r="H21" s="9"/>
       <c r="I21" s="10"/>
       <c r="J21" s="6"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="14"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="13"/>
       <c r="N21" s="10"/>
       <c r="O21" s="5"/>
     </row>
     <row r="22" spans="1:15" ht="13.2">
       <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="69" t="s">
+        <v>49</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1290,9 +1342,15 @@
     </row>
     <row r="23" spans="1:15" ht="13.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="69" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="70">
+        <v>0.255</v>
+      </c>
+      <c r="D23" s="69">
+        <v>0.73499999999999999</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1307,9 +1365,15 @@
     </row>
     <row r="24" spans="1:15" ht="13.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="70">
+        <v>0.255</v>
+      </c>
+      <c r="D24" s="69">
+        <v>0.21</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1324,9 +1388,15 @@
     </row>
     <row r="25" spans="1:15" ht="13.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="69" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="70">
+        <v>1.32</v>
+      </c>
+      <c r="D25" s="69">
+        <v>1.89</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1341,9 +1411,15 @@
     </row>
     <row r="26" spans="1:15" ht="13.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="70">
+        <v>0.9</v>
+      </c>
+      <c r="D26" s="69">
+        <v>2.52</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1358,9 +1434,15 @@
     </row>
     <row r="27" spans="1:15" ht="16.5" customHeight="1">
       <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="69" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="70">
+        <v>0.26</v>
+      </c>
+      <c r="D27" s="69">
+        <v>0.21</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1375,9 +1457,15 @@
     </row>
     <row r="28" spans="1:15" ht="16.5" customHeight="1">
       <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="B28" s="69" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="70">
+        <v>0.1</v>
+      </c>
+      <c r="D28" s="69">
+        <v>0.16800000000000001</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1392,9 +1480,15 @@
     </row>
     <row r="29" spans="1:15" ht="13.2">
       <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C29" s="70">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="D29" s="69">
+        <v>0.42</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1409,9 +1503,15 @@
     </row>
     <row r="30" spans="1:15" ht="13.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="70">
+        <f>SUM(C23:C29)</f>
+        <v>3.3279999999999998</v>
+      </c>
+      <c r="D30" s="69">
+        <f>SUM(D23:D29)</f>
+        <v>6.1529999999999996</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -2410,11 +2510,11 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{BF71C5B3-521D-4416-86F7-C64CF233BE8F}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F2" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>

</xml_diff>